<commit_message>
Sample data changes in Datasheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestPack\WppRegPack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="22" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="27" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="1141">
   <si>
     <t>Description</t>
   </si>
@@ -3463,9 +3463,6 @@
     <t>15969.85</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
     <t>Template Number</t>
   </si>
   <si>
@@ -3481,22 +3478,19 @@
     <t>2/05/2020</t>
   </si>
   <si>
-    <t>1307100147</t>
-  </si>
-  <si>
     <t>2/04/2020</t>
   </si>
   <si>
-    <t>130710010B</t>
-  </si>
-  <si>
     <t>Invoice Journal NO</t>
   </si>
   <si>
-    <t>1307100358</t>
-  </si>
-  <si>
     <t>Vendor Invoice NO</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>130710010C</t>
   </si>
 </sst>
 </file>
@@ -6540,7 +6534,7 @@
   <dimension ref="A1:FK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6751,9 +6745,7 @@
       <c r="A2" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="C2" s="65">
-        <v>1307200446</v>
-      </c>
+      <c r="C2" s="65"/>
       <c r="E2" s="65"/>
       <c r="F2" s="66"/>
       <c r="G2" s="66"/>
@@ -6775,24 +6767,15 @@
       <c r="A5" s="30" t="s">
         <v>452</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>1137</v>
-      </c>
     </row>
     <row r="6" spans="1:167" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="7" spans="1:167" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>1142</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
   </sheetData>
@@ -6843,7 +6826,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
   </sheetData>
@@ -6894,7 +6877,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
   </sheetData>
@@ -7137,7 +7120,7 @@
   </sheetPr>
   <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:K2"/>
     </sheetView>
   </sheetViews>
@@ -8980,7 +8963,7 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -9004,7 +8987,7 @@
         <v>473</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="E1" s="27" t="s">
         <v>463</v>
@@ -9046,16 +9029,16 @@
       </c>
       <c r="B2" s="66"/>
       <c r="C2" s="66" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="D2" s="66" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="E2" s="65" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="F2" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
     </row>
   </sheetData>
@@ -13093,7 +13076,7 @@
         <v>257</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>141</v>
@@ -13221,7 +13204,7 @@
         <v>1307</v>
       </c>
       <c r="C2" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="D2" t="s">
         <v>73</v>
@@ -13519,7 +13502,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13550,7 +13533,7 @@
         <v>126</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>1131</v>
+        <v>1139</v>
       </c>
       <c r="C3" s="30"/>
     </row>

</xml_diff>

<commit_message>
Updated USer Creation sheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GlobalTestSuite_BAU\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="25" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3260" uniqueCount="1426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="1429">
   <si>
     <t>Description</t>
   </si>
@@ -4386,20 +4386,28 @@
     <t>1286_GlobalVendor</t>
   </si>
   <si>
-    <t>125382</t>
-  </si>
-  <si>
     <t>B1286B343</t>
   </si>
   <si>
     <t>125383</t>
+  </si>
+  <si>
+    <t>9/30/2020</t>
+  </si>
+  <si>
+    <t>1286AutomationUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1286-Grey Worldwide Sdn Bhd </t>
+  </si>
+  <si>
+    <t>9/23/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5179,8 +5187,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="2" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="10" width="40.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5279,9 +5287,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="45" width="30.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="26.85546875" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="30.140625" style="45" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -5440,39 +5448,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -5797,9 +5805,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5845,8 +5853,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5893,7 +5901,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5927,9 +5935,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6149,40 +6157,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -6516,9 +6524,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6568,9 +6576,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="47.5703125" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6790,40 +6798,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -7040,12 +7048,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="27.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="23.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="27" width="27.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="51.7109375" collapsed="true"/>
-    <col min="5" max="168" customWidth="true" style="27" width="32.0" collapsed="true"/>
-    <col min="169" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="27.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.140625" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.85546875" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="51.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="168" width="32" style="27" customWidth="1" collapsed="1"/>
+    <col min="169" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:168" x14ac:dyDescent="0.25">
@@ -7370,7 +7378,7 @@
       </c>
       <c r="B16"/>
       <c r="D16" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7874,9 +7882,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7926,7 +7934,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7985,8 +7993,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -8045,8 +8053,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -8105,9 +8113,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="93" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="93" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="93" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="93" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -8164,9 +8172,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="93" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="93" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="93" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="93" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -8223,9 +8231,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="93" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="93" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="93" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="93" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -8285,28 +8293,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -8472,8 +8480,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" style="27" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8681,16 +8689,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="31.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="60.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="59.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="51.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="51.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="27" width="58.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="27" width="57.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="27" width="63.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="45.28515625" collapsed="true"/>
-    <col min="10" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="31" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="59.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="51" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="58.140625" style="27" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="57.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="63.7109375" style="27" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9080,7 +9088,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
+    <col min="2" max="2" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -10254,89 +10262,117 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="23.140625" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.140625" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="46">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>1051</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="47">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>166</v>
       </c>
       <c r="B4" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="47">
+        <v>12869905</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="14" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="14" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="47" t="s">
         <v>835</v>
+      </c>
+      <c r="C9" s="47">
+        <v>1286</v>
       </c>
     </row>
   </sheetData>
@@ -10361,11 +10397,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="60.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="67.42578125" collapsed="true"/>
-    <col min="4" max="9" bestFit="true" customWidth="true" width="87.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="69.42578125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="9" width="87.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="69.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10849,8 +10885,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="31.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="60.140625" collapsed="true"/>
+    <col min="1" max="1" width="31" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10979,7 +11015,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11071,9 +11107,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
@@ -11382,8 +11418,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -11422,8 +11458,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -11469,8 +11505,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11505,8 +11541,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -11562,8 +11598,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11613,7 +11649,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -13667,46 +13703,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
@@ -13930,40 +13966,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -14135,8 +14171,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -14190,8 +14226,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -14245,41 +14281,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -14457,8 +14493,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14502,41 +14538,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -14714,8 +14750,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -14759,8 +14795,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -14870,8 +14906,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14953,8 +14989,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -15097,9 +15133,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -15183,9 +15219,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -15253,9 +15289,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -15323,8 +15359,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -15394,11 +15430,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="7" max="15" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="15" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -15501,7 +15537,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -15542,7 +15578,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -15577,8 +15613,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -15629,13 +15665,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -15710,7 +15746,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -15754,8 +15790,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15921,8 +15957,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -15972,13 +16008,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -16053,7 +16089,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -16097,8 +16133,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -16148,9 +16184,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="24.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -16220,9 +16256,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="24.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -16297,8 +16333,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -16346,10 +16382,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="27" width="22.42578125" collapsed="true"/>
-    <col min="4" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -16432,9 +16468,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -16512,8 +16548,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -16583,8 +16619,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="4" bestFit="true" customWidth="true" width="43.7109375" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="43.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -16933,11 +16969,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -17119,17 +17155,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -17263,17 +17299,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -17442,7 +17478,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17479,17 +17515,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -17602,9 +17638,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="93" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="93" width="35.0" collapsed="true"/>
-    <col min="3" max="16384" style="93" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17645,8 +17681,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17679,9 +17715,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="93" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="93" width="35.0" collapsed="true"/>
-    <col min="3" max="16384" style="93" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -17722,7 +17758,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -17955,9 +17991,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="10.0" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -18013,14 +18049,14 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="4" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18171,7 +18207,7 @@
         <v>979</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>1360</v>
@@ -18185,7 +18221,7 @@
         <v>979</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D12" s="55" t="s">
         <v>1360</v>
@@ -18497,8 +18533,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="14.140625" collapsed="true"/>
-    <col min="2" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -18541,15 +18577,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18630,16 +18666,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -18732,7 +18768,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -19275,13 +19311,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19807,16 +19843,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -19887,49 +19923,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.25">
@@ -20184,49 +20220,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.25">
@@ -20481,9 +20517,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="93" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="93" width="22.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="93" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="93" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.28515625" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -20586,8 +20622,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -20799,10 +20835,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" style="93" width="23.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="93" width="24.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="93" width="22.28515625" collapsed="true"/>
-    <col min="5" max="16384" style="93" width="8.7109375" collapsed="true"/>
+    <col min="1" max="2" width="23" style="93" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="93" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.28515625" style="93" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.7109375" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -20947,9 +20983,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="93" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="93" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="93" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="93" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -21084,10 +21120,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="93" width="22.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="93" width="34.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="93" width="32.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="93" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="22.7109375" style="93" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.140625" style="93" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.5703125" style="93" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.7109375" style="93" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated 1286 opco data
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="25" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="82" activeTab="85"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="1429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3292" uniqueCount="1434">
   <si>
     <t>Description</t>
   </si>
@@ -4149,36 +4149,9 @@
     <t>1286 Finance (TST)</t>
   </si>
   <si>
-    <t>1286 Account Director</t>
-  </si>
-  <si>
-    <t>1286 Admin</t>
-  </si>
-  <si>
-    <t>1286 Basic</t>
-  </si>
-  <si>
-    <t>1286 Biller</t>
-  </si>
-  <si>
     <t>1286 Finance</t>
   </si>
   <si>
-    <t>1286 HR</t>
-  </si>
-  <si>
-    <t>1286 Management</t>
-  </si>
-  <si>
-    <t>1286 Production</t>
-  </si>
-  <si>
-    <t>1286 Project Manager</t>
-  </si>
-  <si>
-    <t>1286 Senior Finance</t>
-  </si>
-  <si>
     <t>1286-Shanghai Ogilvy &amp; Mather Marketing Communications Consulting Co.,Ltd.</t>
   </si>
   <si>
@@ -4341,9 +4314,6 @@
     <t>1286_测试员工自动化</t>
   </si>
   <si>
-    <t>08/31/2020</t>
-  </si>
-  <si>
     <t>1286_AutomationEmpy@gmail.com</t>
   </si>
   <si>
@@ -4353,18 +4323,9 @@
     <t>09/10/2020</t>
   </si>
   <si>
-    <t>37</t>
-  </si>
-  <si>
     <t>Acquisition</t>
   </si>
   <si>
-    <t>1286_AutoClient</t>
-  </si>
-  <si>
-    <t>A1286A0123</t>
-  </si>
-  <si>
     <t>110003</t>
   </si>
   <si>
@@ -4383,12 +4344,6 @@
     <t>AutoGlobalProduct 03September2020 14:29:48</t>
   </si>
   <si>
-    <t>1286_GlobalVendor</t>
-  </si>
-  <si>
-    <t>B1286B343</t>
-  </si>
-  <si>
     <t>125383</t>
   </si>
   <si>
@@ -4402,6 +4357,66 @@
   </si>
   <si>
     <t>9/23/2020</t>
+  </si>
+  <si>
+    <t>1286 Account Director (TST)</t>
+  </si>
+  <si>
+    <t>1286 Admin (TST)</t>
+  </si>
+  <si>
+    <t>1286 Basic (TST)</t>
+  </si>
+  <si>
+    <t>1286 Biller (TST)</t>
+  </si>
+  <si>
+    <t>1286 HR (TST)</t>
+  </si>
+  <si>
+    <t>1286 Management (TST)</t>
+  </si>
+  <si>
+    <t>1286 Production (TST)</t>
+  </si>
+  <si>
+    <t>1286 Project Manager (TST)</t>
+  </si>
+  <si>
+    <t>1286 Senior Finance (TST)</t>
+  </si>
+  <si>
+    <t>A1286A076</t>
+  </si>
+  <si>
+    <t>A1286A064</t>
+  </si>
+  <si>
+    <t>12869905</t>
+  </si>
+  <si>
+    <t>B1286B0082</t>
+  </si>
+  <si>
+    <t>09/28/2020</t>
+  </si>
+  <si>
+    <t>09/07/2020</t>
+  </si>
+  <si>
+    <t>Shanghai Ogilvy &amp; Mather Marketing Communications Consulting Co.,Ltd.</t>
+  </si>
+  <si>
+    <t>9/8/2020（按</t>
+  </si>
+  <si>
+    <t>9/1/2020</t>
+  </si>
+  <si>
+    <t>1286600000</t>
+  </si>
+  <si>
+    <t>9/8/2020</t>
   </si>
 </sst>
 </file>
@@ -4682,7 +4697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4895,6 +4910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5217,7 +5233,7 @@
         <v>867</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
@@ -5261,7 +5277,7 @@
         <v>891</v>
       </c>
       <c r="C5" t="s">
-        <v>1370</v>
+        <v>1361</v>
       </c>
     </row>
   </sheetData>
@@ -5442,8 +5458,8 @@
   </sheetPr>
   <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5828,7 +5844,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>184</v>
@@ -5916,7 +5932,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
   </sheetData>
@@ -5970,7 +5986,7 @@
         <v>832</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1354</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5992,7 +6008,7 @@
         <v>995</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1362</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -6003,7 +6019,7 @@
         <v>996</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1363</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -6036,7 +6052,7 @@
         <v>982</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1366</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6047,7 +6063,7 @@
         <v>983</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1367</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6069,7 +6085,7 @@
         <v>834</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1368</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6080,7 +6096,7 @@
         <v>998</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1364</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -6091,7 +6107,7 @@
         <v>997</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>1365</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6109,7 +6125,7 @@
         <v>984</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>1371</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -6499,7 +6515,7 @@
         <v>922</v>
       </c>
       <c r="AC3" t="s">
-        <v>1392</v>
+        <v>1383</v>
       </c>
       <c r="AD3">
         <v>25</v>
@@ -6554,7 +6570,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -6611,7 +6627,7 @@
         <v>832</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1354</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -6677,7 +6693,7 @@
         <v>982</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1366</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -6688,7 +6704,7 @@
         <v>983</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1367</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6710,7 +6726,7 @@
         <v>834</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1368</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6750,7 +6766,7 @@
         <v>984</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>1371</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7020,7 +7036,7 @@
         <v>1177</v>
       </c>
       <c r="I3" t="s">
-        <v>1397</v>
+        <v>1388</v>
       </c>
       <c r="J3">
         <v>15</v>
@@ -7315,7 +7331,7 @@
       </c>
       <c r="B9"/>
       <c r="D9" t="s">
-        <v>1416</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="10" spans="1:168" x14ac:dyDescent="0.25">
@@ -7324,7 +7340,7 @@
       </c>
       <c r="B10"/>
       <c r="D10" t="s">
-        <v>1417</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="11" spans="1:168" x14ac:dyDescent="0.25">
@@ -7333,7 +7349,7 @@
       </c>
       <c r="B11"/>
       <c r="D11" t="s">
-        <v>1418</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="12" spans="1:168" x14ac:dyDescent="0.25">
@@ -7342,7 +7358,7 @@
       </c>
       <c r="B12"/>
       <c r="D12" t="s">
-        <v>1419</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="13" spans="1:168" x14ac:dyDescent="0.25">
@@ -7351,7 +7367,7 @@
       </c>
       <c r="B13"/>
       <c r="D13" t="s">
-        <v>1420</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="14" spans="1:168" x14ac:dyDescent="0.25">
@@ -7360,7 +7376,7 @@
       </c>
       <c r="B14"/>
       <c r="D14" t="s">
-        <v>1421</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="15" spans="1:168" x14ac:dyDescent="0.25">
@@ -7378,7 +7394,7 @@
       </c>
       <c r="B16"/>
       <c r="D16" t="s">
-        <v>1424</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -7850,19 +7866,19 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>1372</v>
+        <v>1363</v>
       </c>
       <c r="D88"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1373</v>
+        <v>1364</v>
       </c>
       <c r="D89"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>1374</v>
+        <v>1365</v>
       </c>
       <c r="D90"/>
     </row>
@@ -7912,7 +7928,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -8446,7 +8462,7 @@
         <v>1286</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>1355</v>
+        <v>1346</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>1062</v>
@@ -8475,13 +8491,14 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8492,7 +8509,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8508,8 +8525,8 @@
       <c r="B3" s="27" t="s">
         <v>1041</v>
       </c>
-      <c r="C3" s="55" t="s">
-        <v>1412</v>
+      <c r="C3" s="55">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -8681,10 +8698,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8709,7 +8726,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="D1" s="28"/>
       <c r="E1" s="57"/>
@@ -8726,7 +8743,7 @@
         <v>861</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>1407</v>
+        <v>1398</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -8742,7 +8759,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -8757,8 +8774,8 @@
       <c r="B4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>1369</v>
+      <c r="C4" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -8773,8 +8790,8 @@
       <c r="B5" s="14" t="s">
         <v>835</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>1354</v>
+      <c r="C5" s="14" t="s">
+        <v>1360</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -8790,8 +8807,8 @@
       <c r="B6" s="6" t="s">
         <v>832</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>1408</v>
+      <c r="C6" s="6" t="s">
+        <v>1345</v>
       </c>
       <c r="D6"/>
       <c r="E6" s="14"/>
@@ -8807,7 +8824,7 @@
         <v>1046</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>27</v>
+        <v>1427</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -8823,8 +8840,8 @@
       <c r="B8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="87" t="s">
-        <v>1409</v>
+      <c r="C8" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -8839,8 +8856,8 @@
       <c r="B9" s="87" t="s">
         <v>1047</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>30</v>
+      <c r="C9" s="87" t="s">
+        <v>1399</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -8856,7 +8873,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -8873,7 +8890,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -8889,8 +8906,8 @@
       <c r="B12" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>1366</v>
+      <c r="C12" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -8906,8 +8923,8 @@
       <c r="B13" s="6" t="s">
         <v>982</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>1367</v>
+      <c r="C13" s="6" t="s">
+        <v>1357</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -8923,8 +8940,8 @@
       <c r="B14" s="7" t="s">
         <v>983</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>833</v>
+      <c r="C14" s="7" t="s">
+        <v>1358</v>
       </c>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
@@ -8940,8 +8957,8 @@
       <c r="B15" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>1368</v>
+      <c r="C15" s="6" t="s">
+        <v>833</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -8956,8 +8973,8 @@
       <c r="B16" s="7" t="s">
         <v>834</v>
       </c>
-      <c r="C16" s="55" t="s">
-        <v>1355</v>
+      <c r="C16" s="7" t="s">
+        <v>1359</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
@@ -8974,7 +8991,7 @@
         <v>963</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>1355</v>
+        <v>1425</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -8990,8 +9007,8 @@
       <c r="B18" s="55" t="s">
         <v>963</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>170</v>
+      <c r="C18" s="55" t="s">
+        <v>1425</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -9007,8 +9024,8 @@
       <c r="B19" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="53" t="s">
-        <v>1048</v>
+      <c r="C19" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -9023,8 +9040,8 @@
       <c r="B20" s="53" t="s">
         <v>1048</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>40</v>
+      <c r="C20" s="53" t="s">
+        <v>1048</v>
       </c>
       <c r="D20" s="53"/>
       <c r="E20" s="53"/>
@@ -9041,7 +9058,7 @@
         <v>40</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -9057,7 +9074,9 @@
       <c r="B22" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -9065,10 +9084,13 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="17"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -10264,8 +10286,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10295,7 +10317,7 @@
         <v>1051</v>
       </c>
       <c r="C2" t="s">
-        <v>1426</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -10328,7 +10350,7 @@
         <v>832</v>
       </c>
       <c r="C5" t="s">
-        <v>1427</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -10350,7 +10372,7 @@
         <v>1046</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1428</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -10361,7 +10383,7 @@
         <v>1050</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1425</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -10391,8 +10413,8 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10412,7 +10434,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="28"/>
@@ -10430,7 +10452,7 @@
         <v>861</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>1407</v>
+        <v>1398</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -10448,7 +10470,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -10465,8 +10487,8 @@
       <c r="B4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>1369</v>
+      <c r="C4" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -10483,8 +10505,8 @@
       <c r="B5" s="14" t="s">
         <v>835</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>1354</v>
+      <c r="C5" s="14" t="s">
+        <v>1360</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -10501,8 +10523,8 @@
       <c r="B6" s="6" t="s">
         <v>832</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>1408</v>
+      <c r="C6" s="6" t="s">
+        <v>1345</v>
       </c>
       <c r="D6" s="14"/>
       <c r="F6" s="14"/>
@@ -10519,7 +10541,7 @@
         <v>1046</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>27</v>
+        <v>1428</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -10536,8 +10558,8 @@
       <c r="B8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="87" t="s">
-        <v>1409</v>
+      <c r="C8" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -10554,8 +10576,8 @@
       <c r="B9" s="87" t="s">
         <v>1047</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>30</v>
+      <c r="C9" s="87" t="s">
+        <v>1399</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
@@ -10573,7 +10595,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -10591,7 +10613,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -10608,8 +10630,8 @@
       <c r="B12" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>1366</v>
+      <c r="C12" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -10626,8 +10648,8 @@
       <c r="B13" s="6" t="s">
         <v>982</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>1367</v>
+      <c r="C13" s="6" t="s">
+        <v>1357</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -10644,8 +10666,8 @@
       <c r="B14" s="7" t="s">
         <v>983</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>833</v>
+      <c r="C14" s="7" t="s">
+        <v>1358</v>
       </c>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
@@ -10662,8 +10684,8 @@
       <c r="B15" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>1368</v>
+      <c r="C15" s="6" t="s">
+        <v>833</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -10680,8 +10702,8 @@
       <c r="B16" s="7" t="s">
         <v>834</v>
       </c>
-      <c r="C16" s="55" t="s">
-        <v>1355</v>
+      <c r="C16" s="7" t="s">
+        <v>1359</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
@@ -10699,7 +10721,7 @@
         <v>963</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>1355</v>
+        <v>1425</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -10716,8 +10738,8 @@
       <c r="B18" s="55" t="s">
         <v>963</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>170</v>
+      <c r="C18" s="55" t="s">
+        <v>1425</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -10734,8 +10756,8 @@
       <c r="B19" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="53" t="s">
-        <v>1048</v>
+      <c r="C19" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -10752,8 +10774,8 @@
       <c r="B20" s="53" t="s">
         <v>1048</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>40</v>
+      <c r="C20" s="53" t="s">
+        <v>1048</v>
       </c>
       <c r="D20" s="53"/>
       <c r="E20" s="53"/>
@@ -10771,7 +10793,7 @@
         <v>40</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -10788,8 +10810,8 @@
       <c r="B22" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>14</v>
+      <c r="C22" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -10806,8 +10828,8 @@
       <c r="B23" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>1410</v>
+      <c r="C23" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -10825,7 +10847,7 @@
         <v>1046</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>1411</v>
+        <v>1400</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -10835,14 +10857,16 @@
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>1050</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="15" t="s">
+        <v>1401</v>
+      </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -10855,6 +10879,7 @@
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -10865,7 +10890,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -14186,7 +14211,7 @@
         <v>688</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>835</v>
@@ -14807,7 +14832,7 @@
         <v>1319</v>
       </c>
       <c r="C1" s="79" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -14829,7 +14854,7 @@
         <v>1319</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -14851,7 +14876,7 @@
         <v>1319</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -14862,7 +14887,7 @@
         <v>1069</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>1375</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -14918,7 +14943,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -14956,7 +14981,7 @@
         <v>214</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>1413</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -14984,7 +15009,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15012,7 +15037,7 @@
         <v>863</v>
       </c>
       <c r="C2" t="s">
-        <v>1344</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -15023,7 +15048,7 @@
         <v>864</v>
       </c>
       <c r="C3" t="s">
-        <v>1345</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -15034,7 +15059,7 @@
         <v>865</v>
       </c>
       <c r="C4" t="s">
-        <v>1346</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -15045,7 +15070,7 @@
         <v>866</v>
       </c>
       <c r="C5" t="s">
-        <v>1347</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -15056,7 +15081,7 @@
         <v>867</v>
       </c>
       <c r="C6" t="s">
-        <v>1348</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -15067,7 +15092,7 @@
         <v>868</v>
       </c>
       <c r="C7" t="s">
-        <v>1349</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -15078,7 +15103,7 @@
         <v>869</v>
       </c>
       <c r="C8" t="s">
-        <v>1350</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -15089,7 +15114,7 @@
         <v>870</v>
       </c>
       <c r="C9" t="s">
-        <v>1351</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -15100,7 +15125,7 @@
         <v>871</v>
       </c>
       <c r="C10" t="s">
-        <v>1352</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15111,7 +15136,7 @@
         <v>872</v>
       </c>
       <c r="C11" t="s">
-        <v>1353</v>
+        <v>1422</v>
       </c>
     </row>
   </sheetData>
@@ -15128,7 +15153,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15146,7 +15171,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -15168,7 +15193,7 @@
         <v>835</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -15506,16 +15531,16 @@
         <v>1286</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>1405</v>
+        <v>1396</v>
       </c>
       <c r="D3" s="55" t="s">
-        <v>1405</v>
+        <v>1396</v>
       </c>
       <c r="E3" t="s">
-        <v>1406</v>
+        <v>1397</v>
       </c>
       <c r="F3" t="s">
-        <v>1406</v>
+        <v>1397</v>
       </c>
     </row>
   </sheetData>
@@ -16197,7 +16222,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16269,7 +16294,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16396,7 +16421,7 @@
         <v>835</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16438,10 +16463,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>1403</v>
+        <v>1394</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>1404</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -16614,7 +16639,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16645,10 +16670,10 @@
         <v>832</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>1354</v>
+        <v>1345</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1354</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -16659,10 +16684,10 @@
         <v>962</v>
       </c>
       <c r="C3" t="s">
-        <v>1414</v>
+        <v>1348</v>
       </c>
       <c r="D3" t="s">
-        <v>1357</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -16729,10 +16754,10 @@
         <v>944</v>
       </c>
       <c r="C8" t="s">
-        <v>1359</v>
+        <v>1350</v>
       </c>
       <c r="D8" t="s">
-        <v>1359</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -16743,10 +16768,10 @@
         <v>899</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>1415</v>
+        <v>1423</v>
       </c>
       <c r="D9" s="55" t="s">
-        <v>1361</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -16757,10 +16782,10 @@
         <v>899</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>1415</v>
+        <v>1424</v>
       </c>
       <c r="D10" s="55" t="s">
-        <v>1361</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -16869,10 +16894,10 @@
         <v>963</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>1355</v>
+        <v>1425</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>1355</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -16911,10 +16936,10 @@
         <v>964</v>
       </c>
       <c r="C21" t="s">
-        <v>1356</v>
+        <v>1347</v>
       </c>
       <c r="D21" t="s">
-        <v>1356</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -16948,8 +16973,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1"/>
-    <hyperlink ref="C16" r:id="rId2"/>
-    <hyperlink ref="D16" r:id="rId3"/>
+    <hyperlink ref="D16" r:id="rId2"/>
+    <hyperlink ref="C16" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -17435,7 +17460,7 @@
         <v>1286</v>
       </c>
       <c r="E4" t="s">
-        <v>1376</v>
+        <v>1367</v>
       </c>
       <c r="F4" t="s">
         <v>1267</v>
@@ -17447,13 +17472,13 @@
         <v>500</v>
       </c>
       <c r="L4" s="107" t="s">
-        <v>1377</v>
+        <v>1368</v>
       </c>
       <c r="M4" t="s">
         <v>237</v>
       </c>
       <c r="O4" t="s">
-        <v>1378</v>
+        <v>1369</v>
       </c>
       <c r="P4" s="55" t="s">
         <v>1269</v>
@@ -17753,12 +17778,15 @@
   <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:AC3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -17941,36 +17969,90 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D3" t="s">
+        <v>882</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="L3" t="s">
+        <v>932</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="P3" t="s">
+        <v>833</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="U3" t="s">
+        <v>237</v>
+      </c>
+      <c r="V3" t="s">
         <v>1369</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
+      <c r="W3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="X3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>833</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>1197</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18049,14 +18131,16 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18066,7 +18150,7 @@
       <c r="B1">
         <v>1319</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="27">
         <v>1286</v>
       </c>
       <c r="D1">
@@ -18080,11 +18164,11 @@
       <c r="B2" s="6" t="s">
         <v>832</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>1354</v>
+      <c r="C2" s="14" t="s">
+        <v>1345</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>1354</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -18094,7 +18178,7 @@
       <c r="B3" t="s">
         <v>923</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="27" t="s">
         <v>923</v>
       </c>
       <c r="D3" t="s">
@@ -18108,7 +18192,7 @@
       <c r="B4" s="87" t="s">
         <v>924</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="108" t="s">
         <v>924</v>
       </c>
       <c r="D4" s="87" t="s">
@@ -18122,7 +18206,7 @@
       <c r="B5" s="55" t="s">
         <v>978</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>978</v>
       </c>
       <c r="D5" s="55" t="s">
@@ -18136,7 +18220,7 @@
       <c r="B6" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="27" t="s">
         <v>84</v>
       </c>
       <c r="D6" t="s">
@@ -18150,11 +18234,11 @@
       <c r="B7" t="s">
         <v>965</v>
       </c>
-      <c r="C7" t="s">
-        <v>1422</v>
+      <c r="C7" s="27" t="s">
+        <v>1349</v>
       </c>
       <c r="D7" t="s">
-        <v>1358</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -18164,7 +18248,7 @@
       <c r="B8" s="55" t="s">
         <v>896</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="56" t="s">
         <v>896</v>
       </c>
       <c r="D8" s="55" t="s">
@@ -18178,7 +18262,7 @@
       <c r="B9" t="s">
         <v>966</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="27" t="s">
         <v>966</v>
       </c>
       <c r="D9" t="s">
@@ -18192,7 +18276,7 @@
       <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="27" t="s">
         <v>58</v>
       </c>
       <c r="D10" t="s">
@@ -18206,11 +18290,11 @@
       <c r="B11" s="55" t="s">
         <v>979</v>
       </c>
-      <c r="C11" s="55" t="s">
-        <v>1423</v>
+      <c r="C11" s="56" t="s">
+        <v>1426</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>1360</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -18220,11 +18304,11 @@
       <c r="B12" s="55" t="s">
         <v>979</v>
       </c>
-      <c r="C12" s="55" t="s">
-        <v>1423</v>
+      <c r="C12" s="56" t="s">
+        <v>1426</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>1360</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -18234,7 +18318,7 @@
       <c r="B13" t="s">
         <v>931</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="27" t="s">
         <v>931</v>
       </c>
       <c r="D13" t="s">
@@ -18248,7 +18332,7 @@
       <c r="B14" t="s">
         <v>932</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="27" t="s">
         <v>932</v>
       </c>
       <c r="D14" t="s">
@@ -18262,7 +18346,7 @@
       <c r="B15" t="s">
         <v>905</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="27" t="s">
         <v>905</v>
       </c>
       <c r="D15" t="s">
@@ -18276,7 +18360,7 @@
       <c r="B16" t="s">
         <v>936</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="27" t="s">
         <v>936</v>
       </c>
       <c r="D16" t="s">
@@ -18290,7 +18374,7 @@
       <c r="B17" t="s">
         <v>938</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="27" t="s">
         <v>938</v>
       </c>
       <c r="D17" t="s">
@@ -18304,7 +18388,7 @@
       <c r="B18" t="s">
         <v>934</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="27" t="s">
         <v>934</v>
       </c>
       <c r="D18" t="s">
@@ -18318,7 +18402,7 @@
       <c r="B19" s="55" t="s">
         <v>941</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="56" t="s">
         <v>941</v>
       </c>
       <c r="D19" s="55" t="s">
@@ -18332,7 +18416,7 @@
       <c r="B20" t="s">
         <v>934</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="27" t="s">
         <v>934</v>
       </c>
       <c r="D20" t="s">
@@ -18346,7 +18430,7 @@
       <c r="B21" t="s">
         <v>867</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="27" t="s">
         <v>1343</v>
       </c>
       <c r="D21" t="s">
@@ -18360,11 +18444,11 @@
       <c r="B22" t="s">
         <v>944</v>
       </c>
-      <c r="C22" t="s">
-        <v>1359</v>
+      <c r="C22" s="27" t="s">
+        <v>1350</v>
       </c>
       <c r="D22" t="s">
-        <v>1359</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -18374,7 +18458,7 @@
       <c r="B23" t="s">
         <v>914</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="27" t="s">
         <v>914</v>
       </c>
       <c r="D23" t="s">
@@ -18388,7 +18472,7 @@
       <c r="B24" t="s">
         <v>934</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="27" t="s">
         <v>934</v>
       </c>
       <c r="D24" t="s">
@@ -18402,7 +18486,7 @@
       <c r="B25" t="s">
         <v>912</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="27" t="s">
         <v>912</v>
       </c>
       <c r="D25" t="s">
@@ -18416,7 +18500,7 @@
       <c r="B26" t="s">
         <v>949</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="27" t="s">
         <v>949</v>
       </c>
       <c r="D26" t="s">
@@ -18430,7 +18514,7 @@
       <c r="B27">
         <v>3000</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="27">
         <v>3000</v>
       </c>
       <c r="D27">
@@ -18444,7 +18528,7 @@
       <c r="B28">
         <v>300000</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="27">
         <v>300000</v>
       </c>
       <c r="D28">
@@ -18506,14 +18590,13 @@
       <c r="B35" s="55" t="s">
         <v>977</v>
       </c>
-      <c r="C35" s="55"/>
       <c r="D35" s="55"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -18620,12 +18703,12 @@
         <v>164</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>1379</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -18737,19 +18820,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>1393</v>
+        <v>1384</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>1394</v>
+        <v>1385</v>
       </c>
       <c r="D3" s="56" t="s">
-        <v>1395</v>
+        <v>1386</v>
       </c>
       <c r="K3" s="55" t="s">
-        <v>1355</v>
+        <v>1346</v>
       </c>
     </row>
   </sheetData>
@@ -18981,16 +19064,16 @@
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1396</v>
+        <v>1387</v>
       </c>
       <c r="B3" t="s">
         <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>1380</v>
+        <v>1371</v>
       </c>
       <c r="D3" t="s">
-        <v>1381</v>
+        <v>1372</v>
       </c>
       <c r="E3" t="s">
         <v>1019</v>
@@ -19014,10 +19097,10 @@
         <v>988</v>
       </c>
       <c r="L3" t="s">
-        <v>1382</v>
+        <v>1373</v>
       </c>
       <c r="M3" t="s">
-        <v>1383</v>
+        <v>1374</v>
       </c>
       <c r="N3" t="s">
         <v>1098</v>
@@ -19032,19 +19115,19 @@
         <v>1185</v>
       </c>
       <c r="R3" t="s">
-        <v>1384</v>
+        <v>1375</v>
       </c>
       <c r="S3" t="s">
-        <v>1385</v>
+        <v>1376</v>
       </c>
       <c r="T3" t="s">
         <v>990</v>
       </c>
       <c r="U3" t="s">
-        <v>1386</v>
+        <v>1377</v>
       </c>
       <c r="V3" t="s">
-        <v>1387</v>
+        <v>1378</v>
       </c>
       <c r="W3" t="s">
         <v>1100</v>
@@ -19059,7 +19142,7 @@
         <v>1201</v>
       </c>
       <c r="AA3" t="s">
-        <v>1388</v>
+        <v>1379</v>
       </c>
       <c r="AB3" t="s">
         <v>1205</v>
@@ -19068,10 +19151,10 @@
         <v>992</v>
       </c>
       <c r="AD3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="AE3" t="s">
         <v>1380</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>1389</v>
       </c>
       <c r="AF3" t="s">
         <v>1104</v>
@@ -19095,7 +19178,7 @@
         <v>993</v>
       </c>
       <c r="AM3" t="s">
-        <v>1380</v>
+        <v>1371</v>
       </c>
       <c r="AN3" t="s">
         <v>1104</v>
@@ -19122,10 +19205,10 @@
         <v>839</v>
       </c>
       <c r="AV3" t="s">
-        <v>1390</v>
+        <v>1381</v>
       </c>
       <c r="AW3" t="s">
-        <v>1391</v>
+        <v>1382</v>
       </c>
       <c r="AX3" t="s">
         <v>1112</v>
@@ -19149,7 +19232,7 @@
         <v>994</v>
       </c>
       <c r="BE3" t="s">
-        <v>1390</v>
+        <v>1381</v>
       </c>
       <c r="BF3" t="s">
         <v>1104</v>
@@ -19184,13 +19267,13 @@
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="B4" t="s">
-        <v>1397</v>
+        <v>1388</v>
       </c>
       <c r="C4" t="s">
-        <v>1398</v>
+        <v>1389</v>
       </c>
       <c r="D4" t="s">
         <v>1098</v>
@@ -19199,7 +19282,7 @@
         <v>1098</v>
       </c>
       <c r="F4" t="s">
-        <v>1399</v>
+        <v>1390</v>
       </c>
       <c r="G4" t="s">
         <v>1185</v>
@@ -19211,13 +19294,13 @@
         <v>1007</v>
       </c>
       <c r="J4" t="s">
-        <v>1400</v>
+        <v>1391</v>
       </c>
       <c r="K4" t="s">
         <v>249</v>
       </c>
       <c r="L4" t="s">
-        <v>1398</v>
+        <v>1389</v>
       </c>
       <c r="M4" t="s">
         <v>1108</v>
@@ -19226,7 +19309,7 @@
         <v>1108</v>
       </c>
       <c r="O4" t="s">
-        <v>1399</v>
+        <v>1390</v>
       </c>
       <c r="P4" t="s">
         <v>1187</v>
@@ -19238,7 +19321,7 @@
         <v>1007</v>
       </c>
       <c r="S4" t="s">
-        <v>1400</v>
+        <v>1391</v>
       </c>
       <c r="T4"/>
       <c r="U4"/>
@@ -19286,10 +19369,10 @@
       <c r="BK4"/>
       <c r="BL4"/>
       <c r="BM4" t="s">
-        <v>1401</v>
+        <v>1392</v>
       </c>
       <c r="BN4" t="s">
-        <v>1402</v>
+        <v>1393</v>
       </c>
       <c r="BO4" s="55" t="s">
         <v>1189</v>
@@ -19837,8 +19920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19892,19 +19975,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>1369</v>
+        <v>1360</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>1393</v>
+        <v>1384</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>1394</v>
+        <v>1385</v>
       </c>
       <c r="D2" s="56" t="s">
-        <v>1395</v>
+        <v>1386</v>
       </c>
       <c r="K2" s="55" t="s">
-        <v>1355</v>
+        <v>1346</v>
       </c>
     </row>
   </sheetData>
@@ -20565,7 +20648,7 @@
         <v>1339</v>
       </c>
       <c r="C5" s="94" t="s">
-        <v>1375</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -20617,7 +20700,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20656,7 +20739,7 @@
         <v>832</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1354</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -20678,7 +20761,7 @@
         <v>995</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1362</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -20689,7 +20772,7 @@
         <v>996</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1363</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -20722,7 +20805,7 @@
         <v>982</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>1366</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -20733,7 +20816,7 @@
         <v>983</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1367</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -20755,7 +20838,7 @@
         <v>834</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1368</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -20766,7 +20849,7 @@
         <v>998</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>1364</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -20777,7 +20860,7 @@
         <v>997</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>1365</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -20795,7 +20878,7 @@
         <v>984</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>1371</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -21026,7 +21109,7 @@
         <v>1339</v>
       </c>
       <c r="C3" s="94" t="s">
-        <v>1375</v>
+        <v>1366</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -21183,7 +21266,7 @@
         <v>1284</v>
       </c>
       <c r="C6" s="94" t="s">
-        <v>1375</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updaed User Creation Sheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="82" activeTab="85"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620" firstSheet="28" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -4353,9 +4353,6 @@
     <t>1286AutomationUser</t>
   </si>
   <si>
-    <t xml:space="preserve">1286-Grey Worldwide Sdn Bhd </t>
-  </si>
-  <si>
     <t>9/23/2020</t>
   </si>
   <si>
@@ -4417,6 +4414,9 @@
   </si>
   <si>
     <t>9/8/2020</t>
+  </si>
+  <si>
+    <t>Company</t>
   </si>
 </sst>
 </file>
@@ -8701,7 +8701,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8824,7 +8824,7 @@
         <v>1046</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -8991,7 +8991,7 @@
         <v>963</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -9008,7 +9008,7 @@
         <v>963</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -10286,8 +10286,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10322,7 +10322,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>1</v>
+        <v>1433</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>835</v>
@@ -10350,7 +10350,7 @@
         <v>832</v>
       </c>
       <c r="C5" t="s">
-        <v>1412</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -10372,7 +10372,7 @@
         <v>1046</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -10541,7 +10541,7 @@
         <v>1046</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -10721,7 +10721,7 @@
         <v>963</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -10739,7 +10739,7 @@
         <v>963</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -15037,7 +15037,7 @@
         <v>863</v>
       </c>
       <c r="C2" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -15048,7 +15048,7 @@
         <v>864</v>
       </c>
       <c r="C3" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -15059,7 +15059,7 @@
         <v>865</v>
       </c>
       <c r="C4" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -15070,7 +15070,7 @@
         <v>866</v>
       </c>
       <c r="C5" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -15092,7 +15092,7 @@
         <v>868</v>
       </c>
       <c r="C7" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -15103,7 +15103,7 @@
         <v>869</v>
       </c>
       <c r="C8" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -15114,7 +15114,7 @@
         <v>870</v>
       </c>
       <c r="C9" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -15125,7 +15125,7 @@
         <v>871</v>
       </c>
       <c r="C10" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15136,7 +15136,7 @@
         <v>872</v>
       </c>
       <c r="C11" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
     </row>
   </sheetData>
@@ -16768,7 +16768,7 @@
         <v>899</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="D9" s="55" t="s">
         <v>1352</v>
@@ -16782,7 +16782,7 @@
         <v>899</v>
       </c>
       <c r="C10" s="55" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D10" s="55" t="s">
         <v>1352</v>
@@ -16894,7 +16894,7 @@
         <v>963</v>
       </c>
       <c r="C18" s="55" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D18" s="55" t="s">
         <v>1346</v>
@@ -17973,25 +17973,25 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="D3" t="s">
         <v>882</v>
       </c>
       <c r="E3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F3" t="s">
         <v>1430</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1431</v>
       </c>
       <c r="G3" t="s">
         <v>1410</v>
       </c>
       <c r="H3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="I3" t="s">
         <v>1432</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1433</v>
       </c>
       <c r="J3" t="s">
         <v>1267</v>
@@ -18021,10 +18021,10 @@
         <v>1301</v>
       </c>
       <c r="S3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="T3" t="s">
         <v>1432</v>
-      </c>
-      <c r="T3" t="s">
-        <v>1433</v>
       </c>
       <c r="U3" t="s">
         <v>237</v>
@@ -18291,7 +18291,7 @@
         <v>979</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>1351</v>
@@ -18305,7 +18305,7 @@
         <v>979</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="D12" s="55" t="s">
         <v>1351</v>
@@ -19920,7 +19920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added JobClosure Updated script and Test Data Files
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Modified\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\OneDrive - Cognizant\Documents\GlobalTestSuite Project\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="109" activeTab="112"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -124,28 +124,29 @@
     <sheet name="Time_Material_Invocing" sheetId="96" r:id="rId110"/>
     <sheet name="InvoicingWriteOff" sheetId="69" r:id="rId111"/>
     <sheet name="InvoicingCarryForward" sheetId="71" r:id="rId112"/>
-    <sheet name="CreateGlobalBrand" sheetId="105" r:id="rId113"/>
-    <sheet name="CreateGlobalProduct" sheetId="106" r:id="rId114"/>
-    <sheet name="CreateCompanyClient" sheetId="107" r:id="rId115"/>
-    <sheet name="CreateCompanyBrand" sheetId="108" r:id="rId116"/>
-    <sheet name="CreateCompanyProduct" sheetId="109" r:id="rId117"/>
-    <sheet name="AmendCompanyClient" sheetId="110" r:id="rId118"/>
-    <sheet name="AmendCompanyBrand" sheetId="111" r:id="rId119"/>
-    <sheet name="AmendCompanyProduct" sheetId="112" r:id="rId120"/>
-    <sheet name="AmendGlobalClient" sheetId="113" r:id="rId121"/>
-    <sheet name="AmendGlobalBrand" sheetId="114" r:id="rId122"/>
-    <sheet name="AmendGlobalProduct" sheetId="115" r:id="rId123"/>
-    <sheet name="BlockCompanyProduct" sheetId="121" r:id="rId124"/>
-    <sheet name="BlockCompanyBrand" sheetId="118" r:id="rId125"/>
-    <sheet name="BlockCompanyClient" sheetId="119" r:id="rId126"/>
-    <sheet name="BlockGlobalProduct" sheetId="120" r:id="rId127"/>
-    <sheet name="BlockGlobalBrand" sheetId="47" r:id="rId128"/>
-    <sheet name="BlockGlobalClient" sheetId="48" r:id="rId129"/>
-    <sheet name="CreateCompanyVendor" sheetId="123" r:id="rId130"/>
-    <sheet name="AmendGlobalVendor" sheetId="116" r:id="rId131"/>
-    <sheet name="AmendCompanyVendor" sheetId="117" r:id="rId132"/>
-    <sheet name="BlockGlobalVendor" sheetId="122" r:id="rId133"/>
-    <sheet name="BlockCompanyVendor" sheetId="124" r:id="rId134"/>
+    <sheet name="CombinedInvoice" sheetId="140" r:id="rId113"/>
+    <sheet name="CreateGlobalBrand" sheetId="105" r:id="rId114"/>
+    <sheet name="CreateGlobalProduct" sheetId="106" r:id="rId115"/>
+    <sheet name="CreateCompanyClient" sheetId="107" r:id="rId116"/>
+    <sheet name="CreateCompanyBrand" sheetId="108" r:id="rId117"/>
+    <sheet name="CreateCompanyProduct" sheetId="109" r:id="rId118"/>
+    <sheet name="AmendCompanyClient" sheetId="110" r:id="rId119"/>
+    <sheet name="AmendCompanyBrand" sheetId="111" r:id="rId120"/>
+    <sheet name="AmendCompanyProduct" sheetId="112" r:id="rId121"/>
+    <sheet name="AmendGlobalClient" sheetId="113" r:id="rId122"/>
+    <sheet name="AmendGlobalBrand" sheetId="114" r:id="rId123"/>
+    <sheet name="AmendGlobalProduct" sheetId="115" r:id="rId124"/>
+    <sheet name="BlockCompanyProduct" sheetId="121" r:id="rId125"/>
+    <sheet name="BlockCompanyBrand" sheetId="118" r:id="rId126"/>
+    <sheet name="BlockCompanyClient" sheetId="119" r:id="rId127"/>
+    <sheet name="BlockGlobalProduct" sheetId="120" r:id="rId128"/>
+    <sheet name="BlockGlobalBrand" sheetId="47" r:id="rId129"/>
+    <sheet name="BlockGlobalClient" sheetId="48" r:id="rId130"/>
+    <sheet name="CreateCompanyVendor" sheetId="123" r:id="rId131"/>
+    <sheet name="AmendGlobalVendor" sheetId="116" r:id="rId132"/>
+    <sheet name="AmendCompanyVendor" sheetId="117" r:id="rId133"/>
+    <sheet name="BlockGlobalVendor" sheetId="122" r:id="rId134"/>
+    <sheet name="BlockCompanyVendor" sheetId="124" r:id="rId135"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -157,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5502" uniqueCount="1708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5513" uniqueCount="1709">
   <si>
     <t>Description</t>
   </si>
@@ -5282,6 +5283,9 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>1221200124</t>
   </si>
 </sst>
 </file>
@@ -7490,7 +7494,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8899,6 +8903,78 @@
 
 <file path=xl/worksheets/sheet113.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="102" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="102" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="102" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="106" t="s">
+        <v>952</v>
+      </c>
+      <c r="C1" s="106" t="s">
+        <v>953</v>
+      </c>
+      <c r="D1" s="106" t="s">
+        <v>954</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="104" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="102">
+        <v>1284</v>
+      </c>
+      <c r="B2" s="106" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C2" s="106" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D2" s="106" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F2" s="105" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="102">
+        <v>1221</v>
+      </c>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="F3" s="105" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet114.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9077,7 +9153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet114.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet115.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -9248,7 +9324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet115.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet116.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -9434,7 +9510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet116.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet117.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -9636,7 +9712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet117.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -9838,7 +9914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet118.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -9899,86 +9975,6 @@
       </c>
       <c r="B5" s="105"/>
       <c r="C5" s="105"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet119.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" style="102" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="28.28515625" style="102" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="102" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
-        <v>658</v>
-      </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="105" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="105" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
-        <v>837</v>
-      </c>
-      <c r="B4" s="105" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C4" s="105" t="s">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="s">
-        <v>835</v>
-      </c>
-      <c r="B5" s="105"/>
-      <c r="C5" s="105"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
-        <v>659</v>
-      </c>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="102" t="s">
-        <v>660</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10188,7 +10184,7 @@
         <v>1182</v>
       </c>
       <c r="C4" s="105" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -10200,14 +10196,14 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="102" t="s">
-        <v>1180</v>
+        <v>659</v>
       </c>
       <c r="B6" s="109"/>
       <c r="C6" s="109"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="102" t="s">
-        <v>1170</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -10217,6 +10213,86 @@
 </file>
 
 <file path=xl/worksheets/sheet121.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="102" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="28.28515625" style="102" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="102" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="102" t="s">
+        <v>658</v>
+      </c>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="102" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="105" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="102" t="s">
+        <v>837</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C4" s="105" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="102" t="s">
+        <v>835</v>
+      </c>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="102" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="102" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -10299,7 +10375,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -10408,7 +10484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -10517,7 +10593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet124.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet125.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -10577,7 +10653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet125.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet126.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -10637,7 +10713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet126.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet127.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -10686,7 +10762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet127.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet128.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -10746,7 +10822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet128.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet129.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -10801,56 +10877,6 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>660</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet129.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="72" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -10901,6 +10927,56 @@
 
 <file path=xl/worksheets/sheet130.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet131.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11081,7 +11157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet131.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet132.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -11168,7 +11244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet132.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet133.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -11244,7 +11320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet133.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet134.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -11292,7 +11368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet134.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet135.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -13973,8 +14049,8 @@
   </sheetPr>
   <dimension ref="A1:FI141"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14356,8 +14432,8 @@
       <c r="A24" t="s">
         <v>159</v>
       </c>
-      <c r="B24" t="s">
-        <v>1690</v>
+      <c r="B24" s="105" t="s">
+        <v>1708</v>
       </c>
       <c r="C24" s="105"/>
     </row>
@@ -15473,7 +15549,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating Client Management Scripts
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\Modified\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\OneDrive - Cognizant\Documents\WPP Global TestScripts\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="119" activeTab="122"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5782" uniqueCount="1781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5813" uniqueCount="1780">
   <si>
     <t>Description</t>
   </si>
@@ -5472,24 +5472,6 @@
     <t>st1</t>
   </si>
   <si>
-    <t>110540</t>
-  </si>
-  <si>
-    <t>1301_AutoClient 15March2021 17:54:12</t>
-  </si>
-  <si>
-    <t>110540001</t>
-  </si>
-  <si>
-    <t>AutoGlobalBrand 15March2021 17:54:12</t>
-  </si>
-  <si>
-    <t>110540001001</t>
-  </si>
-  <si>
-    <t>AutoGlobalProduct 15March2021 17:54:12</t>
-  </si>
-  <si>
     <t>B1301Z013</t>
   </si>
   <si>
@@ -5509,13 +5491,27 @@
   </si>
   <si>
     <t>AutoGlobalProduct 15March2021 19:33:50</t>
+  </si>
+  <si>
+    <t>Geometry Ogilvy Japan GK</t>
+  </si>
+  <si>
+    <t>1301 Finance</t>
+  </si>
+  <si>
+    <t>108269001</t>
+  </si>
+  <si>
+    <t>108269001001</t>
+  </si>
+  <si>
+    <t>Geometry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6309,8 +6305,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="2" max="5" bestFit="true" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="40.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6407,10 +6403,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="81" width="32.5703125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="81" width="19.0" collapsed="true"/>
-    <col min="5" max="16384" style="81" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="23" style="81" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.5703125" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="19" style="81" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.7109375" style="81" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -6538,9 +6534,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="35.0" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6600,7 +6596,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -6901,20 +6897,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="23.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="32.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="101" width="13.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="101" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="101" width="23.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="101" width="12.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="101" width="19.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="101" width="13.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="101" width="21.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="101" width="23.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="101" width="11.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="101" width="18.85546875" collapsed="true"/>
-    <col min="14" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.5703125" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="21.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.85546875" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -7077,18 +7073,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="22.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="20.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="101" width="17.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="101" width="16.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="101" width="15.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="101" width="17.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="101" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="101" width="20.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="101" width="17.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="101" width="15.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="101" width="13.42578125" collapsed="true"/>
-    <col min="12" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.5703125" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" style="101" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.5703125" style="101" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17" style="101" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" style="101" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.42578125" style="101" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.140625" style="101" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" style="101" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -7200,16 +7196,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="27" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="27" width="11.0" collapsed="true"/>
-    <col min="11" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" style="27" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7304,7 +7300,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7356,7 +7352,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -8017,10 +8013,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -8093,13 +8089,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="101" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="101" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="101" width="13.5703125" collapsed="true"/>
-    <col min="5" max="5" style="101" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="101" width="17.85546875" collapsed="true"/>
-    <col min="7" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="101" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="101" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -8171,15 +8167,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="27" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="24.5703125" collapsed="true"/>
-    <col min="10" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" style="27" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8311,10 +8307,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="81" width="32.5703125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="81" width="17.0" collapsed="true"/>
-    <col min="5" max="16384" style="81" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="81" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.5703125" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17" style="81" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="8.7109375" style="81" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -8455,10 +8451,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="10.0" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8506,18 +8502,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="27" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="27" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="27" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="23.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="27" width="22.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="27" width="30.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="28.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="27" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="27" width="23.7109375" collapsed="true"/>
-    <col min="12" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="21" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" style="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.140625" style="27" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.7109375" style="27" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -8644,16 +8640,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="30.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -8758,49 +8754,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.25">
@@ -9132,49 +9128,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="56" max="56" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.25">
@@ -9505,13 +9501,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="101" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="101" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="19.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="101" width="13.5703125" collapsed="true"/>
-    <col min="5" max="5" style="101" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="101" width="17.85546875" collapsed="true"/>
-    <col min="7" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="101" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="101" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -9577,13 +9573,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" style="101" width="9.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="101" width="19.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="101" width="13.5703125" collapsed="true"/>
-    <col min="6" max="10" style="101" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="101" width="17.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="9.140625" style="101" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="10" width="9.140625" style="101" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -9688,7 +9684,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" style="101" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -10154,9 +10150,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="18.0" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="103" width="35.0" collapsed="true"/>
-    <col min="4" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="35" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -10334,10 +10330,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="22.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="81" width="34.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="81" width="32.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="81" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="22.7109375" style="81" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.140625" style="81" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.5703125" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.7109375" style="81" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -10484,9 +10480,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="18.0" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="103" width="35.0" collapsed="true"/>
-    <col min="4" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="35" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -10647,20 +10643,20 @@
 
 <file path=xl/worksheets/sheet121.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="19.5703125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="30.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.5703125" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="30.7109375" style="101" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>5</v>
       </c>
@@ -10670,8 +10666,11 @@
       <c r="C1" s="71">
         <v>1221</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="71">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="101" t="s">
         <v>49</v>
       </c>
@@ -10681,15 +10680,19 @@
       <c r="C2" s="101" t="s">
         <v>1578</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="101" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="101" t="s">
         <v>658</v>
       </c>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="104"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>820</v>
       </c>
@@ -10699,8 +10702,11 @@
       <c r="C4" s="101" t="s">
         <v>1496</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="101" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="101" t="s">
         <v>178</v>
       </c>
@@ -10710,8 +10716,11 @@
       <c r="C5" s="104" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="104" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="101" t="s">
         <v>1172</v>
       </c>
@@ -10721,8 +10730,11 @@
       <c r="C6" s="104">
         <v>1221</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="104">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="101" t="s">
         <v>177</v>
       </c>
@@ -10732,8 +10744,11 @@
       <c r="C7" s="101" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="101" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="101" t="s">
         <v>871</v>
       </c>
@@ -10743,8 +10758,11 @@
       <c r="C8" s="101" t="s">
         <v>1597</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="101" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="101" t="s">
         <v>26</v>
       </c>
@@ -10754,8 +10772,11 @@
       <c r="C9" s="75" t="s">
         <v>1173</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="75" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="101" t="s">
         <v>1174</v>
       </c>
@@ -10765,8 +10786,11 @@
       <c r="C10" s="104" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="104" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="101" t="s">
         <v>1175</v>
       </c>
@@ -10776,8 +10800,11 @@
       <c r="C11" s="101" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="101" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="101" t="s">
         <v>875</v>
       </c>
@@ -10787,8 +10814,11 @@
       <c r="C12" s="101" t="s">
         <v>1176</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="101" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="101" t="s">
         <v>1177</v>
       </c>
@@ -10798,8 +10828,11 @@
       <c r="C13" s="101" t="s">
         <v>1581</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="101" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="101" t="s">
         <v>873</v>
       </c>
@@ -10809,8 +10842,11 @@
       <c r="C14" s="101" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="101" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="101" t="s">
         <v>1178</v>
       </c>
@@ -10818,6 +10854,9 @@
         <v>1179</v>
       </c>
       <c r="C15" s="104" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D15" s="104" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -10825,28 +10864,29 @@
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>
+    <hyperlink ref="D9" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet122.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="19.5703125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="30.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.5703125" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="30.7109375" style="101" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>5</v>
       </c>
@@ -10856,8 +10896,11 @@
       <c r="C1" s="71">
         <v>1221</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="71">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="101" t="s">
         <v>49</v>
       </c>
@@ -10867,15 +10910,19 @@
       <c r="C2" s="101" t="s">
         <v>1578</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="101" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="101" t="s">
         <v>658</v>
       </c>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="104"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>659</v>
       </c>
@@ -10885,13 +10932,16 @@
       <c r="C4" s="105" t="s">
         <v>1499</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="104" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="101" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="101" t="s">
         <v>660</v>
       </c>
@@ -10901,8 +10951,11 @@
       <c r="C6" s="104" t="s">
         <v>1496</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="101" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="101" t="s">
         <v>178</v>
       </c>
@@ -10912,8 +10965,11 @@
       <c r="C7" s="104" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="104" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="101" t="s">
         <v>1172</v>
       </c>
@@ -10923,8 +10979,11 @@
       <c r="C8" s="104">
         <v>1221</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="104">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="101" t="s">
         <v>177</v>
       </c>
@@ -10934,8 +10993,11 @@
       <c r="C9" s="101" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="101" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="101" t="s">
         <v>871</v>
       </c>
@@ -10945,8 +11007,11 @@
       <c r="C10" s="101" t="s">
         <v>1597</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="101" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="101" t="s">
         <v>26</v>
       </c>
@@ -10956,8 +11021,11 @@
       <c r="C11" s="75" t="s">
         <v>1173</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="75" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="101" t="s">
         <v>1174</v>
       </c>
@@ -10967,8 +11035,11 @@
       <c r="C12" s="104" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="104" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="101" t="s">
         <v>1175</v>
       </c>
@@ -10978,8 +11049,11 @@
       <c r="C13" s="101" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="101" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="101" t="s">
         <v>875</v>
       </c>
@@ -10989,8 +11063,11 @@
       <c r="C14" s="101" t="s">
         <v>1176</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="101" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="101" t="s">
         <v>1177</v>
       </c>
@@ -11000,8 +11077,11 @@
       <c r="C15" s="101" t="s">
         <v>1581</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="101" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="101" t="s">
         <v>873</v>
       </c>
@@ -11011,8 +11091,11 @@
       <c r="C16" s="101" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="101" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="101" t="s">
         <v>1178</v>
       </c>
@@ -11020,6 +11103,9 @@
         <v>1179</v>
       </c>
       <c r="C17" s="104" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D17" s="104" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -11027,28 +11113,29 @@
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1"/>
     <hyperlink ref="C11" r:id="rId2"/>
+    <hyperlink ref="D11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet123.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="19.5703125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="30.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.5703125" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="30.7109375" style="101" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>5</v>
       </c>
@@ -11058,8 +11145,11 @@
       <c r="C1" s="71">
         <v>1221</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="71">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="101" t="s">
         <v>49</v>
       </c>
@@ -11069,15 +11159,19 @@
       <c r="C2" s="101" t="s">
         <v>1578</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="101" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="101" t="s">
         <v>658</v>
       </c>
       <c r="B3" s="104"/>
       <c r="C3" s="104"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="104"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>1180</v>
       </c>
@@ -11087,13 +11181,16 @@
       <c r="C4" s="105" t="s">
         <v>1498</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="104" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="101" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="101" t="s">
         <v>1170</v>
       </c>
@@ -11103,8 +11200,11 @@
       <c r="C6" s="104" t="s">
         <v>1497</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="104" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="101" t="s">
         <v>178</v>
       </c>
@@ -11114,8 +11214,11 @@
       <c r="C7" s="104" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="104" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="101" t="s">
         <v>1172</v>
       </c>
@@ -11125,8 +11228,11 @@
       <c r="C8" s="104">
         <v>1221</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="104">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="101" t="s">
         <v>177</v>
       </c>
@@ -11136,8 +11242,11 @@
       <c r="C9" s="101" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="101" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="101" t="s">
         <v>871</v>
       </c>
@@ -11147,8 +11256,11 @@
       <c r="C10" s="101" t="s">
         <v>1597</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="101" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="101" t="s">
         <v>26</v>
       </c>
@@ -11158,8 +11270,11 @@
       <c r="C11" s="75" t="s">
         <v>1173</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="75" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="101" t="s">
         <v>1174</v>
       </c>
@@ -11169,8 +11284,11 @@
       <c r="C12" s="104" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="104" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="101" t="s">
         <v>1175</v>
       </c>
@@ -11180,8 +11298,11 @@
       <c r="C13" s="101" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="101" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="101" t="s">
         <v>875</v>
       </c>
@@ -11191,8 +11312,11 @@
       <c r="C14" s="101" t="s">
         <v>1176</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="101" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="101" t="s">
         <v>1177</v>
       </c>
@@ -11202,8 +11326,11 @@
       <c r="C15" s="101" t="s">
         <v>1581</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="101" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="101" t="s">
         <v>873</v>
       </c>
@@ -11213,8 +11340,11 @@
       <c r="C16" s="101" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="101" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="101" t="s">
         <v>1178</v>
       </c>
@@ -11222,6 +11352,9 @@
         <v>1179</v>
       </c>
       <c r="C17" s="104" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D17" s="104" t="s">
         <v>1179</v>
       </c>
     </row>
@@ -11229,9 +11362,10 @@
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1"/>
     <hyperlink ref="C11" r:id="rId2"/>
+    <hyperlink ref="D11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -11245,9 +11379,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="23.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="28.28515625" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="28.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11313,9 +11447,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="23.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="28.28515625" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="28.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11393,9 +11527,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="23.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="28.28515625" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="28.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11473,9 +11607,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="17.5703125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="101" width="29.140625" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="29.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -11556,9 +11690,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="17.5703125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="101" width="39.0" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="39" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -11665,9 +11799,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="17.5703125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="101" width="39.0" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="39" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -11774,9 +11908,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="101" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11814,9 +11948,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="19.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.42578125" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -11874,9 +12008,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="24.85546875" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -11934,9 +12068,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="13.0" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11983,9 +12117,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="31.85546875" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12046,9 +12180,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="10.0" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12109,8 +12243,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="14.140625" collapsed="true"/>
-    <col min="2" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12156,9 +12290,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="18.85546875" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="101" width="35.0" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.85546875" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="35" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -12338,9 +12472,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="25.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="25.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12425,9 +12559,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="101" width="25.85546875" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="25.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12501,9 +12635,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="25.85546875" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12549,9 +12683,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="101" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -12589,9 +12723,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="101" width="18.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -12635,17 +12769,17 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+    <sheetView topLeftCell="F6" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" hidden="true" style="101" width="43.85546875" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" hidden="true" width="43.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="6" max="9" bestFit="true" customWidth="true" style="101" width="43.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.85546875" style="101" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="43.7109375" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="9" width="43.85546875" style="101" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -12906,7 +13040,7 @@
         <v>1582</v>
       </c>
       <c r="I9" s="104" t="s">
-        <v>1774</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -12935,7 +13069,7 @@
         <v>1582</v>
       </c>
       <c r="I10" s="104" t="s">
-        <v>1774</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -13376,12 +13510,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="35.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="27" width="35.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="35.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="103" width="35.7109375" collapsed="true"/>
-    <col min="7" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="35" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="35.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -13970,11 +14104,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="32.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="101" width="32.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="101" width="57.0" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="57" style="101" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -14339,11 +14473,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="45" width="30.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="26.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="27" width="31.0" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="103" width="31.0" collapsed="true"/>
-    <col min="6" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="30.140625" style="45" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="31" style="103" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -14655,48 +14789,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="6" max="6" style="27" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" style="27" width="9.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="27" width="6.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" style="27" width="9.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" style="27" width="9.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" style="27" width="9.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" style="27" width="9.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" style="27" width="9.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="38" max="38" style="27" width="9.140625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" style="27" width="13.42578125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="27" width="14.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="42" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="27" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.140625" style="27" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.140625" style="27" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="9.140625" style="27" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.140625" style="27" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.140625" style="27" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.140625" style="27" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="9.140625" style="27" collapsed="1"/>
+    <col min="39" max="39" width="13.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="14.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
@@ -15328,10 +15462,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="39.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="23.7109375" collapsed="true"/>
-    <col min="3" max="164" customWidth="true" style="27" width="32.0" collapsed="true"/>
-    <col min="165" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="39.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.7109375" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="164" width="32" style="27" customWidth="1" collapsed="1"/>
+    <col min="165" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:165" x14ac:dyDescent="0.25">
@@ -15534,7 +15668,7 @@
         <v>1583</v>
       </c>
       <c r="D2" t="s">
-        <v>1775</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="3" spans="1:165" x14ac:dyDescent="0.25">
@@ -15548,7 +15682,7 @@
         <v>1584</v>
       </c>
       <c r="D3" t="s">
-        <v>1776</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="4" spans="1:165" x14ac:dyDescent="0.25">
@@ -15562,7 +15696,7 @@
         <v>1585</v>
       </c>
       <c r="D4" t="s">
-        <v>1777</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="5" spans="1:165" x14ac:dyDescent="0.25">
@@ -15576,7 +15710,7 @@
         <v>1586</v>
       </c>
       <c r="D5" t="s">
-        <v>1778</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="6" spans="1:165" x14ac:dyDescent="0.25">
@@ -15590,7 +15724,7 @@
         <v>1587</v>
       </c>
       <c r="D6" t="s">
-        <v>1779</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="7" spans="1:165" x14ac:dyDescent="0.25">
@@ -15604,7 +15738,7 @@
         <v>1588</v>
       </c>
       <c r="D7" t="s">
-        <v>1780</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="8" spans="1:165" x14ac:dyDescent="0.25">
@@ -16525,9 +16659,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="103" customFormat="1" x14ac:dyDescent="0.25">
@@ -16908,9 +17042,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -16983,9 +17117,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -17056,9 +17190,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.25">
@@ -17604,7 +17738,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -17773,11 +17907,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="45.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="101" width="32.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.28515625" style="101" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -18104,49 +18238,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" style="27" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" style="27" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="27" width="6.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" style="27" width="9.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" style="27" width="9.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" style="27" width="9.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="31" max="31" style="27" width="9.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" style="27" width="9.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" style="27" width="9.140625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="27" width="13.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="27" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="43" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.140625" style="27" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="27" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.140625" style="27" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9.140625" style="27" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.140625" style="27" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.140625" style="27" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="9.140625" style="27" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="9.140625" style="27" collapsed="1"/>
+    <col min="40" max="40" width="13.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -18664,10 +18798,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18738,11 +18872,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="47.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="101" width="45.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="101" width="32.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.140625" style="101" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.28515625" style="101" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -19068,40 +19202,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -19480,7 +19614,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
+    <col min="2" max="2" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -20659,10 +20793,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -20733,11 +20867,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="45.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="101" width="32.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.28515625" style="101" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -21055,49 +21189,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" style="27" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" style="27" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="27" width="6.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" style="27" width="9.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" style="27" width="9.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" style="27" width="9.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="31" max="31" style="27" width="9.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" style="27" width="9.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" style="27" width="9.140625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="27" width="13.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="27" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="43" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.140625" style="27" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="27" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.140625" style="27" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9.140625" style="27" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.140625" style="27" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.140625" style="27" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="9.140625" style="27" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="9.140625" style="27" collapsed="1"/>
+    <col min="40" max="40" width="13.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -21615,10 +21749,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -21683,12 +21817,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="101" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="101" width="34.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="101" width="45.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="101" width="32.28515625" collapsed="true"/>
-    <col min="6" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34" style="101" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.140625" style="101" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -22017,49 +22151,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="103" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="103" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" style="103" width="9.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" style="103" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="103" width="6.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" style="103" width="9.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" style="103" width="9.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" style="103" width="9.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="31" max="31" style="103" width="9.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" style="103" width="9.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" style="103" width="9.140625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="103" width="13.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="103" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="103" width="11.7109375" collapsed="true"/>
-    <col min="43" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.140625" style="103" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="103" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.85546875" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.140625" style="103" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="9.140625" style="103" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="9.140625" style="103" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.140625" style="103" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="9.140625" style="103" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="9.140625" style="103" collapsed="1"/>
+    <col min="40" max="40" width="13.42578125" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -22576,10 +22710,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="6.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="103" width="11.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="6.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -22712,7 +22846,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -22786,8 +22920,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -22864,7 +22998,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -24915,8 +25049,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -24990,9 +25124,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="81" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="81" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="81" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="81" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25066,9 +25200,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="81" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="81" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="81" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="81" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25128,9 +25262,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="81" width="16.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="81" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="81" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.28515625" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="8.7109375" style="81" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -25193,30 +25327,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="22.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="27" width="14.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="27" width="10.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="12.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="27" width="10.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="27" width="19.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="27" width="10.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="27" width="19.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="27" width="10.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="27" width="19.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="27" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="27" width="10.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="27" width="13.140625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="27" width="20.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="27" width="11.5703125" collapsed="true"/>
-    <col min="24" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5703125" style="27" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5703125" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="20.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -25423,9 +25557,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="32.140625" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -25466,9 +25600,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="45.5703125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -25512,9 +25646,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="27" width="29.140625" collapsed="true"/>
-    <col min="5" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="29.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -25570,9 +25704,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="19.0" collapsed="true"/>
-    <col min="5" max="5" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -25870,9 +26004,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="18.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -25934,10 +26068,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="4" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="101" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -26179,9 +26313,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="18.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -26249,16 +26383,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="31.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="60.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="59.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="51.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="51.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="103" width="51.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="27" width="57.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="27" width="63.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="45.28515625" collapsed="true"/>
-    <col min="10" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="31" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="59.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="51" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.85546875" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="57.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="63.7109375" style="27" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -26814,9 +26948,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="24.140625" collapsed="true"/>
-    <col min="2" max="5" customWidth="true" style="103" width="23.140625" collapsed="true"/>
-    <col min="6" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="23.140625" style="103" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -26991,11 +27125,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="87.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="87.5703125" collapsed="true"/>
-    <col min="4" max="6" bestFit="true" customWidth="true" width="87.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="69.42578125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="87.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="87.5703125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="87.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="69.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27392,9 +27526,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="31.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="60.140625" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="31" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27458,9 +27592,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="15.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="26.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.5703125" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.28515625" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27526,46 +27660,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
@@ -27877,40 +28011,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -28098,8 +28232,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -28159,8 +28293,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -28220,8 +28354,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28387,42 +28521,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="101" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="101" width="22.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="101" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="101" width="11.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="101" width="11.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="101" width="11.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="101" width="11.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="101" width="11.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="101" width="11.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="101" width="12.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="101" width="13.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="101" width="10.7109375" collapsed="true"/>
-    <col min="36" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="101" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.85546875" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="11.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="11.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="11.140625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="13.28515625" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.7109375" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -28609,43 +28743,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="27" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="38" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -28851,9 +28985,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -28909,43 +29043,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="27" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="27" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="27" width="11.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="27" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="27" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="38" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="27" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -29153,9 +29287,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -29211,43 +29345,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="103" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="103" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="103" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="103" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="38" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="103" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" style="103" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -29467,9 +29601,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -29525,43 +29659,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="103" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="103" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="103" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="103" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="38" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="103" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" style="103" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -29766,43 +29900,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="103" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="15.42578125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="103" width="15.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="103" width="11.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="103" width="22.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="103" width="11.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="103" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="103" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="103" width="10.7109375" collapsed="true"/>
-    <col min="38" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="103" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.42578125" style="103" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.85546875" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="11.140625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
@@ -30007,9 +30141,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -30061,10 +30195,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="101" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="101" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="11.0" collapsed="true"/>
-    <col min="4" max="16384" style="101" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" style="101" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" style="101" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="101" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -30141,9 +30275,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="103" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="103" width="11.0" collapsed="true"/>
-    <col min="3" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -30198,11 +30332,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="24.7109375" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" style="27" width="22.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="103" width="22.5703125" collapsed="true"/>
-    <col min="7" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="22.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.5703125" style="103" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -30384,11 +30518,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="3" max="4" style="27" width="9.140625" collapsed="true"/>
-    <col min="5" max="6" style="103" width="9.140625" collapsed="true"/>
-    <col min="7" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="27" collapsed="1"/>
+    <col min="5" max="6" width="9.140625" style="103" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30515,11 +30649,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.42578125" collapsed="true"/>
-    <col min="3" max="4" style="27" width="9.140625" collapsed="true"/>
-    <col min="5" max="6" style="103" width="9.140625" collapsed="true"/>
-    <col min="7" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="27" collapsed="1"/>
+    <col min="5" max="6" width="9.140625" style="103" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -30646,11 +30780,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" style="27" width="9.140625" collapsed="true"/>
-    <col min="4" max="5" style="103" width="9.140625" collapsed="true"/>
-    <col min="6" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="27" collapsed="1"/>
+    <col min="4" max="5" width="9.140625" style="103" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -30762,11 +30896,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" style="27" width="9.140625" collapsed="true"/>
-    <col min="4" max="5" style="103" width="9.140625" collapsed="true"/>
-    <col min="6" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.140625" style="27" collapsed="1"/>
+    <col min="4" max="5" width="9.140625" style="103" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -30882,12 +31016,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="27" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="7" max="15" bestFit="true" customWidth="true" style="27" width="16.7109375" collapsed="true"/>
-    <col min="16" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" style="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="15" width="16.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -31025,8 +31159,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="2" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -31067,8 +31201,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="2" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -31115,9 +31249,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="27" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="21.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -31171,7 +31305,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="103" width="9.140625" collapsed="true"/>
+    <col min="1" max="16384" width="9.140625" style="103" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -31235,13 +31369,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -31325,9 +31459,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="33.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -31478,10 +31612,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="15.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="101" width="15.42578125" collapsed="true"/>
-    <col min="4" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.42578125" style="101" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -31629,14 +31763,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="10" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.85546875" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" style="27" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -31733,8 +31867,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="2" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -31790,9 +31924,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="27" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="21.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -31854,14 +31988,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="27" width="25.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="27" width="15.85546875" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="27" width="12.0" collapsed="true"/>
-    <col min="10" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="15.85546875" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" style="27" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="12" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" style="27" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -31960,8 +32094,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="2" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -32017,9 +32151,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="27" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="27" width="21.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" style="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -32081,11 +32215,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="24.42578125" collapsed="true"/>
-    <col min="3" max="4" style="27" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" style="103" width="9.140625" collapsed="true"/>
-    <col min="6" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="27" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="103" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -32170,10 +32304,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="81" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="81" width="22.28515625" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" style="81" width="19.140625" collapsed="true"/>
-    <col min="6" max="16384" style="81" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="81" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.28515625" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="19.140625" style="81" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="8.7109375" style="81" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -32300,9 +32434,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="27.5703125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -32356,9 +32490,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="24.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -32453,11 +32587,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="20.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="27" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="27" width="15.7109375" collapsed="true"/>
-    <col min="5" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="20.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" style="27" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -32579,17 +32713,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -32838,17 +32972,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -33094,7 +33228,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -33146,18 +33280,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -33340,9 +33474,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="35.0" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="18" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -33396,9 +33530,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="27" width="11.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="27" width="10.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="27" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.85546875" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="27" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Invoice MPL's and Reports
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_CHN_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="161" activeTab="164"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7501" uniqueCount="2045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7502" uniqueCount="2046">
   <si>
     <t>Description</t>
   </si>
@@ -6499,6 +6499,9 @@
   </si>
   <si>
     <t>2021-02</t>
+  </si>
+  <si>
+    <t>C:\GlobalTestSuiteAutomation\WppRegpack\MPLReports\Critical_Regression\China\1301\Print Invoice EditingSample.pdf</t>
   </si>
 </sst>
 </file>
@@ -14191,7 +14194,7 @@
   <dimension ref="A1:BO7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19251,7 +19254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -19704,8 +19707,8 @@
   </sheetPr>
   <dimension ref="A1:FH212"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C203" sqref="C203"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20095,7 +20098,7 @@
       <c r="A24" t="s">
         <v>159</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="102" t="s">
         <v>2005</v>
       </c>
       <c r="C24" s="99" t="s">
@@ -20607,7 +20610,9 @@
       <c r="A76" t="s">
         <v>1391</v>
       </c>
-      <c r="B76" s="99"/>
+      <c r="B76" s="99" t="s">
+        <v>2045</v>
+      </c>
       <c r="C76" t="s">
         <v>1801</v>
       </c>

</xml_diff>